<commit_message>
kaban, journal et doc
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal-Theo-Pasquier.xlsx
+++ b/documentation/3_1_Journal-Theo-Pasquier.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/theo_pasquier_studentfr_ch/Documents/3eme année/306/projet/306-G1-Piloter_un_robot_phidget_a_distance/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7DF3038-D1B9-4AEA-80C6-BC78B5C4E01A}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9295D16E-A2B8-44EF-88BB-B41E35C4CA0D}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -96,6 +96,24 @@
   </si>
   <si>
     <t>J'ai travaillé un peu lentement sur le cahier des charges ce qui fait que je n'ai même pas pu encore commencer à faire le planning sur le projet mais juste analyser comment le faire. Je me dois de travailler plus vite pour le prochain Sprint.</t>
+  </si>
+  <si>
+    <t>Effectuer le planning</t>
+  </si>
+  <si>
+    <t>modifier cahier des charges</t>
+  </si>
+  <si>
+    <t>modifier cahier des charges en fonction des remarques du client</t>
+  </si>
+  <si>
+    <t>modifier le planning</t>
+  </si>
+  <si>
+    <t>travailler sur le côté développement du projet</t>
+  </si>
+  <si>
+    <t>Cette semaine c'est bien passée, au début j'étais un peu stressé par le fait de faire une réunion avec le client et lui présenter le cahier des charges ainsi que le business case mais tout c'est bien passée, il n'y a pas eu beaucoup de modification à faire alors je me suis dit que j'avais fait un bon travail de ce côté-ci. Au niveau du planning j'ai eu plus de facilité à le faire mais j'ai quand même reçu quelque remarque sur ce dernier. Au niveau du développement du projet j'ai été assez peu efficace comparé à mes collègues mais je pense que je leur ai été assez utile en leur donnant des conseils ou alors en leur donnant des remaques constructive sur ce qu'ils pourraient améliorer.</t>
   </si>
 </sst>
 </file>
@@ -436,100 +454,100 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1167,7 +1185,7 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane ySplit="1" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1218,7 +1236,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36">
+      <c r="A6" s="26">
         <v>45996</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -1230,35 +1248,35 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="18" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1271,45 +1289,67 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="13">
+        <v>46003</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="8"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="8"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="8"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1318,47 +1358,49 @@
       </c>
       <c r="D18" s="9">
         <f>SUM(D13:D17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1371,43 +1413,43 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1420,43 +1462,43 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1469,43 +1511,43 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="15"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="15"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
+      <c r="A46" s="14"/>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1518,43 +1560,43 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="23"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="15"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="15"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="15"/>
+      <c r="A53" s="14"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1567,43 +1609,43 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="26"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="24"/>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="17"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="15"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="19"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="15"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="15"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
+      <c r="A60" s="14"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1616,43 +1658,43 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="26"/>
+      <c r="A61" s="25"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="17"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="15"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
+      <c r="A63" s="14"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="15"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="19"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="15"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="19"/>
+      <c r="A65" s="14"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="18"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="15"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
+      <c r="A66" s="14"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="18"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="15"/>
+      <c r="A67" s="14"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -1665,43 +1707,43 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="15"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="22"/>
+      <c r="A68" s="14"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="16"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="15"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="19"/>
+      <c r="A70" s="14"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="18"/>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="15"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="19"/>
+      <c r="A71" s="14"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="18"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="15"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="19"/>
+      <c r="A72" s="14"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="15"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="19"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="18"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="15"/>
+      <c r="A74" s="14"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1714,43 +1756,43 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="23"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="26"/>
+      <c r="A75" s="25"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="24"/>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="17"/>
+      <c r="A76" s="13"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="15"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="19"/>
+      <c r="A77" s="14"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="18"/>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="15"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="19"/>
+      <c r="A78" s="14"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="15"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="19"/>
+      <c r="A79" s="14"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="18"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="19"/>
+      <c r="A80" s="14"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="18"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
+      <c r="A81" s="14"/>
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -1763,10 +1805,10 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="26"/>
+      <c r="A82" s="25"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="24"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
@@ -1776,53 +1818,51 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>3.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="13" t="s">
+      <c r="A84" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="A62:A68"/>
     <mergeCell ref="B62:C62"/>
@@ -1839,38 +1879,40 @@
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -1985,26 +2027,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -2217,10 +2239,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2239,20 +2292,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
journal, planning + doc
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal-Theo-Pasquier.xlsx
+++ b/documentation/3_1_Journal-Theo-Pasquier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/theo_pasquier_studentfr_ch/Documents/3eme année/306/projet/306-G1-Piloter_un_robot_phidget_a_distance/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60137694-28D7-4A8A-92F9-C5F18151EB31}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A72ECE4-B1B2-4FA2-B674-8E623FBE24E0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>J'ai beaucoup avancé au niveau de la documentation jusqu'à en avoir tellement marre que j'ai été chercher des problèmes rencontrés dans le code effectués par mes collègues. Je suis content du travail effectué même si parfois j'ai manqué un peu d'attention.</t>
+  </si>
+  <si>
+    <t>traduction et implémentation du guide utilisateur</t>
+  </si>
+  <si>
+    <t>Journée très longue car faire de la documentation, quelle qu'elle soit pendant 5h c'est long ennuyant et embêtant. Heureusement que Andrei avait besoin de mon aide pour la traduction et l'implémentation du guide utilisateur pour le clavier. Je fûs distrait par l'extérieur plusieurs fois durant la journée pour manque de motivation à faire la documentation.</t>
   </si>
 </sst>
 </file>
@@ -490,6 +496,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -526,72 +536,68 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -874,6 +880,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1227,9 +1237,9 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40:D40"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1242,85 +1252,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="31"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28">
+      <c r="A6" s="36">
         <v>45996</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1333,67 +1343,67 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
+      <c r="A13" s="14">
         <v>46003</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="15"/>
+      <c r="B17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1406,59 +1416,59 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13">
+      <c r="A20" s="14">
         <v>46009</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="23"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1471,63 +1481,63 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="19" t="s">
+      <c r="A26" s="15"/>
+      <c r="B26" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13">
+      <c r="A27" s="14">
         <v>46010</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="16"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="7">
         <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17" t="s">
+      <c r="A29" s="15"/>
+      <c r="B29" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="18"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="18"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1540,7 +1550,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="27"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="24" t="s">
         <v>27</v>
       </c>
@@ -1548,47 +1558,47 @@
       <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13">
+      <c r="A34" s="14">
         <v>46030</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="16"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="17" t="s">
+      <c r="A35" s="15"/>
+      <c r="B35" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="18"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1601,7 +1611,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="27"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="24" t="s">
         <v>30</v>
       </c>
@@ -1609,37 +1619,47 @@
       <c r="D40" s="26"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="7"/>
+      <c r="A41" s="14">
+        <v>46031</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="17"/>
+      <c r="D41" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="8"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="18"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="18"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1648,47 +1668,49 @@
       </c>
       <c r="D46" s="9">
         <f>SUM(D41:D45)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="27"/>
-      <c r="B47" s="24"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="23"/>
+      <c r="B47" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="C47" s="25"/>
       <c r="D47" s="26"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="18"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="19"/>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="18"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="19"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="19"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1701,43 +1723,43 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="27"/>
+      <c r="A54" s="23"/>
       <c r="B54" s="24"/>
       <c r="C54" s="25"/>
       <c r="D54" s="26"/>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="17"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="19"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="19"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="19"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="18"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="19"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="14"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1750,43 +1772,43 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="27"/>
+      <c r="A61" s="23"/>
       <c r="B61" s="24"/>
       <c r="C61" s="25"/>
       <c r="D61" s="26"/>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="17"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="19"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="18"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="19"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="18"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="19"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="18"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="19"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="14"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -1799,43 +1821,43 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="22"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="13"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="16"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="17"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="18"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="19"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="18"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="19"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="18"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="19"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1848,43 +1870,43 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="27"/>
+      <c r="A75" s="23"/>
       <c r="B75" s="24"/>
       <c r="C75" s="25"/>
       <c r="D75" s="26"/>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="13"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="16"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="17"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="14"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="18"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="19"/>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="14"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="18"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="19"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="18"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="19"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="18"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="19"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="14"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -1897,7 +1919,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="27"/>
+      <c r="A82" s="23"/>
       <c r="B82" s="24"/>
       <c r="C82" s="25"/>
       <c r="D82" s="26"/>
@@ -1910,19 +1932,85 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>24.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="38" t="s">
+      <c r="A84" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="38"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="A84:D84"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="B13:C13"/>
@@ -1939,72 +2027,6 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -2128,6 +2150,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -2340,17 +2373,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
   <ds:schemaRefs>
@@ -2360,6 +2382,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
+    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2376,17 +2411,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
-    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>